<commit_message>
[ADD]csv to exel converter
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,318 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>roberto Santiago</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>+93910966393</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Tatiana</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>+93919059173</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>roberto Santiago</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>+93910966392</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>padre</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>+93654987245</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>sdds</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>+9332323242342</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>sdkn</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Andorra</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>+37632323242342</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Andorra</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>+376323232423411</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thiciana Rocha </t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>+351913895289</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-07-11 03:40:15</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>roberto Santiago</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>+93910966393</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-07-11 03:40:15</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Tatiana</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>+93919059173</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-07-11 03:40:15</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>roberto Santiago</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>+93910966392</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-07-11 03:40:15</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>padre</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>+93654987245</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-07-11 03:40:15</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>sdds</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>+9332323242342</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-07-11 03:40:15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>sdkn</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Andorra</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>+37632323242342</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-07-11 03:40:15</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Andorra</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>+376323232423411</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-07-11 03:40:15</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thiciana Rocha </t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>+351913895289</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
[ADD] create exel file function
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,340 +443,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-07-11 02:58:24</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>nawerwsdf</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Botswana</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>+2676542342342</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>roberto Santiago</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Afghanistan</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>+93910966393</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Tatiana</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Afghanistan</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>+93919059173</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>roberto Santiago</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Afghanistan</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>+93910966392</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>padre</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Afghanistan</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>+93654987245</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>sdds</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Afghanistan</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>+9332323242342</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>sdkn</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Andorra</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>+37632323242342</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>teste</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Andorra</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>+376323232423411</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Thiciana Rocha </t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Portugal</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>+351913895289</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2024-07-11 03:40:15</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>roberto Santiago</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Afghanistan</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>+93910966393</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2024-07-11 03:40:15</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Tatiana</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Afghanistan</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>+93919059173</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2024-07-11 03:40:15</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>roberto Santiago</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Afghanistan</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>+93910966392</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2024-07-11 03:40:15</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>padre</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Afghanistan</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>+93654987245</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2024-07-11 03:40:15</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>sdds</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Afghanistan</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>+9332323242342</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2024-07-11 03:40:15</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>sdkn</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Andorra</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>+37632323242342</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2024-07-11 03:40:15</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>teste</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Andorra</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>+376323232423411</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2024-07-11 03:40:15</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Thiciana Rocha </t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Portugal</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>+351913895289</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] add new rec. has been added a possibility to add new recs in google drive for users witch are note coders
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,6 +443,28 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-07-12 16:41:23</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TestAaron Isac</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>+351924676500</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] visual de site, footer
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,6 +531,138 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-08-06 12:14:18</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">leonardo </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>+9398765432</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-06 16:24:13</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Boris Isac</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Algeria</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>+21398787777777</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-08-06 16:44:50</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>wrewerew</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Bhutan</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>+975654321</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-08-06 16:53:59</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>barbara</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Cameroon</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>+237654987654</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-08-06 16:54:56</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>wer</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>+8634</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-08-06 16:55:31</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>wer</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>+86343</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] the gold print html, css files
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -663,6 +663,314 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-08-07 12:31:33</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>boris</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Benin</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>+2294545455</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-08-07 12:42:41</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>boris</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Bolivia</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>+5914545455</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-08-07 14:30:47</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>pai natal</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>+93777</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-08-07 14:34:02</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Bolivia</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>+591999</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-08-07 14:45:55</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Bolivia</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>+5919999</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-08-07 14:49:23</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Bolivia</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>+59199991</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-08-07 14:58:30</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>qqq</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>+93001100</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-08-07 15:00:06</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>qqq</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>+930011001</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-08-07 15:00:20</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>qqq</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>+9300110011</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-08-07 15:00:42</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>qqq</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>+93001100110</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-08-07 15:02:55</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>+931</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-08-07 15:03:25</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>+9310</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-08-07 16:41:29</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>jhg</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>+93887788</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-08-07 16:45:02</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>boris</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>+933211654987654321</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>